<commit_message>
Flipped cutting planes. Works with all existing tests and use cases.
</commit_message>
<xml_diff>
--- a/Examples/Studio/FemurConstraints/FemurConstraints.xlsx
+++ b/Examples/Studio/FemurConstraints/FemurConstraints.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="162">
   <si>
     <t>name</t>
   </si>
@@ -140,6 +140,156 @@
     <t>value</t>
   </si>
   <si>
+    <t>alignment_enabled</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>alignment_method</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>antialias</t>
+  </si>
+  <si>
+    <t>pad</t>
+  </si>
+  <si>
+    <t>pad_value</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>fastmarching</t>
+  </si>
+  <si>
+    <t>blur</t>
+  </si>
+  <si>
+    <t>blur_sigma</t>
+  </si>
+  <si>
+    <t>2.000000</t>
+  </si>
+  <si>
+    <t>isolate</t>
+  </si>
+  <si>
+    <t>fill_holes</t>
+  </si>
+  <si>
+    <t>fill_mesh_holes</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>antialias_amount</t>
+  </si>
+  <si>
+    <t>groom_output_prefix</t>
+  </si>
+  <si>
+    <t>groomed1</t>
+  </si>
+  <si>
+    <t>convert_to_mesh</t>
+  </si>
+  <si>
+    <t>mesh_smooth</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_method</t>
+  </si>
+  <si>
+    <t>Laplacian</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_laplacian_iterations</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_laplacian_relaxation</t>
+  </si>
+  <si>
+    <t>1.000000</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_windowed_sinc_iterations</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_windowed_sinc_passband</t>
+  </si>
+  <si>
+    <t>0.050000</t>
+  </si>
+  <si>
+    <t>crop</t>
+  </si>
+  <si>
+    <t>reflect</t>
+  </si>
+  <si>
+    <t>reflect_column</t>
+  </si>
+  <si>
+    <t>reflect_choice</t>
+  </si>
+  <si>
+    <t>reflect_axis</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>resample</t>
+  </si>
+  <si>
+    <t>isotropic</t>
+  </si>
+  <si>
+    <t>iso_spacing</t>
+  </si>
+  <si>
+    <t>0.000000</t>
+  </si>
+  <si>
+    <t>spacing</t>
+  </si>
+  <si>
+    <t>0 0 0</t>
+  </si>
+  <si>
+    <t>remesh</t>
+  </si>
+  <si>
+    <t>remesh_percent_mode</t>
+  </si>
+  <si>
+    <t>remesh_percent</t>
+  </si>
+  <si>
+    <t>75.000000</t>
+  </si>
+  <si>
+    <t>remesh_num_vertices</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>remesh_gradation</t>
+  </si>
+  <si>
+    <t>skip_grooming</t>
+  </si>
+  <si>
+    <t>groom_all_domains_the_same</t>
+  </si>
+  <si>
     <t>value_1</t>
   </si>
   <si>
@@ -158,9 +308,6 @@
     <t>initial_relative_weighting</t>
   </si>
   <si>
-    <t>0.050000</t>
-  </si>
-  <si>
     <t>iterations_per_split</t>
   </si>
   <si>
@@ -170,9 +317,6 @@
     <t>multiscale</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>multiscale_particles</t>
   </si>
   <si>
@@ -213,9 +357,6 @@
   </si>
   <si>
     <t>procrustes_interval</t>
-  </si>
-  <si>
-    <t>10</t>
   </si>
   <si>
     <t>procrustes_rotation_translation</t>
@@ -279,12 +420,12 @@
     <t>zoom_state</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>version</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>reconstruction_clusters</t>
   </si>
   <si>
@@ -334,9 +475,6 @@
   </si>
   <si>
     <t>train_decay_learning_rate</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
   <si>
     <t>train_epochs</t>
@@ -825,7 +963,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C37"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
@@ -836,7 +974,403 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -858,162 +1392,162 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1035,50 +1569,50 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1100,10 +1634,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1125,26 +1659,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1166,106 +1700,106 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>154</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1279,19 +1813,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="E1" t="s">
-        <v>115</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>